<commit_message>
New translations extracted_quests.xlsx (French)
</commit_message>
<xml_diff>
--- a/fr/extracted_quests.xlsx
+++ b/fr/extracted_quests.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="254">
   <si>
     <t>Texte Japonais</t>
   </si>
@@ -27,11 +27,29 @@
 好きらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">Tazzi, the Skill Master's apprentice in the
+Alltrades Abbey, asked me to find the owner
+of the book "Profound Puff-Puff" in the
+castle town of the true Kingdom of Arahagiro
+and get the book for him!　The owner of the
+book is a dark and gloomy man named Jiméjito.
+Apparently, the owner of the book likes dark
+and gloomy places.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ジュレットの町にいる　武闘家ヤーンから
 ガウラドに呼びだされているので
 ランガーオ山地にある　ロンダの氷穴の奥
 ガラガの穴に来てほしい！　と頼まれた。
 ヤーンとは　現地で会うことになっている。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martial Artist Yarn, in Julet House, has
+summoned me to Gaurad, and asked me to come
+to Garaga Hole, behind the Rhonda Ice Cave in
+the Langao Mountains!　He asked me to come to
+the Galaga Hole in the Rongda Ice Hole in the
+Langao Mountains. I am to meet Yarn there.</t>
   </si>
   <si>
     <t xml:space="preserve">ガウラドの正体は　超天道士を倒すために
@@ -42,6 +60,16 @@
 グララという女オーガに　話をつけてあるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Gaurad's true identity was that of a monster
+from Demon World who came to defeat the
+Chotenkyoji. Instead of Yarn, he fought
+Warrior Demon Gaurad and defeated him. Yarn
+asked me to compete with him at the Coliseum
+to see what I can find out.　He was asked to
+fight at the Colosseum. It seems that he has
+already talked to a female ogre named Grala.</t>
+  </si>
+  <si>
     <t xml:space="preserve">赤いずきんの女性　コリスに頼まれて
 オオカミ退治を　することになった。
 月の守り神を呼ぶために　月見団子を
@@ -50,6 +78,14 @@
 月見のしずくを　手に入れよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Coris, the woman in the red hood, asked me to
+help her kill the wolves. She wanted to make
+Moon Viewing Dumplings to call the Moon
+Guardian, so we went to Moonlight Plaza
+outside Folmonti Village to get Moon Viewing
+Drops from Lunar Pond.</t>
+  </si>
+  <si>
     <t xml:space="preserve">赤いずきんの女性　コリスに頼まれて
 オオカミ退治を　することになった。
 退治に使う　伝説の銃ススキラーを　作るため
@@ -58,6 +94,15 @@
 銀のススキを　手に入れよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Coris, a woman in a red hood, asked him to
+kill the wolves. To make the legendary gun,
+Susuki, which is used to exterminate wolves,
+you must get Silver Grass from Susukino, who
+appears when you fight Basarana in Sunset
+Meadow and other places in Eltona Continent.
+Get it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">赤いずきんの女性　コリスに頼まれて
 オオカミ退治を　することになった。
 退治に使う　伝説の銃ススキラーを　作るため
@@ -66,16 +111,41 @@
 コリスに　届けよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Coris, the woman in the red hood, has asked
+me to kill the wolves. I received some Silver
+Grass to make the legendary gun, Suskiller,
+which I will use to kill the wolves, and I
+will deliver it to Coris at the Church in
+Folmonti Village.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 真のレンダーシアの　{color=yellow}真のローヌ樹林帯{reset}にいる
 {color=yellow}トリカトラプス{reset}を　１５匹　討伐してほしい！
 現在　０匹　倒している。</t>
   </si>
   <si>
+    <t xml:space="preserve">~Request from Monster Strike Force~ I want
+you to kill
+{color=yellow}Trikaceratops{reset} in
+{color=yellow}True Rhone Forest Belt{reset}
+in True Lendersia! I want you to take down 15
+of them! 　 Currently, 0 of them have been
+killed.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 真のレンダーシアの　{color=yellow}真のローヌ樹林帯{reset}にいる
 {color=yellow}トリカトラプス{reset}を　１５匹　討伐してほしい！
 現在　６匹　倒している。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~Request from Monster Strike Force~ I want
+you to kill
+{color=yellow}Trikaceratops{reset} in
+{color=yellow}True Rhone Forest Belt{reset}
+in True Lendersia! I want you to take down 15
+of them! 　 I've killed 6 of them so far.</t>
   </si>
   <si>
     <t xml:space="preserve">港町レンドア南の　船舶管理局にいる
@@ -85,10 +155,24 @@
 と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">I need the Luring Extract that Charm Bats in
+Becon Valley, Ogreed Continent drop from
+Clerk Jackal at Ship Bureau, South Port Town
+Lendor. I'm in Bekong Canyon on the Orgreid
+Continent. I was asked to get it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 エルトナ大陸の　{color=yellow}落陽の草原{reset}にいる
 {color=yellow}グリンバングル{reset}を　２０匹　討伐してほしい！
 現在　０匹　倒している。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~Request from Monster Strike Force Force~
+I want you to take out 20 Sbonce in Eltona
+Continent's {color=yellow}Sunset Meadow
+{reset}! I want you to take down 20 of them!
+ Currently, 0 of them have been killed.</t>
   </si>
   <si>
     <t xml:space="preserve">メギストリスの都の　噴水公園にいる
@@ -99,10 +183,24 @@
 と言われた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Prove your fashionable senses and get
+yourself a Kisekae doll by wearing Trend Hat
+in fashionable colors from Perere, the self-
+proclaimed fashion critic on the City of
+Megistris fountain.</t>
+  </si>
+  <si>
     <t xml:space="preserve">アラハギーロ王国の宝物庫で　カギ師グラーネから
 開かずの小箱を　メギストリス城の宝物庫にいる
 ネジロに届けてくれ！　と頼まれた。
 ネジロに　会いにいこう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deliver the Unopened Small Box from the
+keymaster Grane at the treasury of the
+Kingdom of Al-Ahagiro to Nejiro at the
+treasury of Megistris Castle!　 Let's go see
+Nejiro.</t>
   </si>
   <si>
     <t xml:space="preserve">偽りの　アラハギーロ城下町で　セラフィから
@@ -113,6 +211,14 @@
 サリュウコツを　集めて　セラフィに渡そう。</t>
   </si>
   <si>
+    <t xml:space="preserve">falseGather medicine materials for the
+townspeople from Seraphi in Al-AhagiroCastle
+Town!　 Collect Rhone Carrot at the south end
+of falseRhone Forest Belt. falseCollect Sand
+Bone from Dragon Zombie at the east desert of
+Al-Ahagiro Region and give it to Seraphi.</t>
+  </si>
+  <si>
     <t xml:space="preserve">妖精図書館の管理人　妖精ミモリーに頼まれ
 誰かの記憶が記された　不思議な本の中に入ると
 セラニーは　リィンという少女の姿に
@@ -121,16 +227,36 @@
 狙っているようだ。神殿の入口を探してみよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Mimori, the caretaker of the Fairy Library,
+asks Serany to enter a mysterious book that
+contains someone's memories, and Serany is
+transformed into a girl named Lynn. Lynn
+seems to be after the treasure of the ruins
+called Night Temple, so let's find the
+entrance to the temple.</t>
+  </si>
+  <si>
     <t xml:space="preserve">不思議の魔塔で　管理人をしているという
 ガチャコッコの　チャコロットから
 塔の中にあらわれた　魔物を退治して
 封印された扉を　解放するように　頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Chacolot of Clockwork Cuckoo, the caretaker
+of Mysterious Tower, asked me to kill the
+demon that appeared in the tower and free the
+sealed door.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ヴェリナード城下町の　カーメロから
 リーネと一緒に　豪華客船のパーティーに
 出席してもらえないか？　と頼まれた。
 さっそく　リーネに話しかけてみよう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could you and Renee from Karmelo in Verinard
+Castle Town attend a party on a luxury cruise
+ship?　 Let's talk to Renee right away.</t>
   </si>
   <si>
     <t xml:space="preserve">グレン城にある　武器鍛冶ギルドで
@@ -140,6 +266,13 @@
 実際に　武器鍛冶に挑戦してみよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">At the Weaponsmith Guild in Glen Castle,
+Guildmaster Rasedo gave me a trial to become
+a weaponsmith. Let's check out the
+weaponsmithing equipment and try our hand at
+weaponsmithing.</t>
+  </si>
+  <si>
     <t xml:space="preserve">エンドールという町からやってきた
 トルネコという商人の依頼で
 妻と息子に宛てた手紙を　郵便局に届けた。
@@ -147,6 +280,13 @@
 報告しよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">I delivered a letter to my wife and son to
+the Post Office at the request of a merchant
+named Torneko from a town called Endor. I'll
+let you know if I see Torneko again at Magic
+Maze.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ヴェリナード領南の　海辺の交易所で　ソーネから
 美容院で使える　新色の開発のため
 ヴェリナード領南の　ホタテワラビーが
@@ -154,6 +294,13 @@
 手に入れてください！　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Get a Silver Scallop, sometimes dropped by
+Verinard South's Scallop Wallaby, from Sonet
+at the Beach Trading Post in Verinard South
+for the development of new colors for the
+salon!</t>
+  </si>
+  <si>
     <t xml:space="preserve">港町レンドア北にある　道具鍛冶ギルドで
 マスター・バレクスから　道具鍛冶職人に
 なるための試練を　受けることになった。
@@ -161,11 +308,25 @@
 内容を覚えたら　バレクスに話しかけよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">At the Toolsmith Guild in North Port Lendor,
+Guildmaster Barex gave me a trial on how to
+become a toolsmith. After learning the
+contents of the recipe book Beginner
+Toolsmithing, I talked to Barex.</t>
+  </si>
+  <si>
     <t xml:space="preserve">港町レンドア北にある　道具鍛冶ギルドで
 マスター・バレクスから　道具鍛冶職人に
 なるための試練を　受けることになった。
 道具鍛冶用の設備をしらべて
 実際に　道具鍛冶に挑戦してみよう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guildmaster Barex at the Toolsmith Guild in
+North Port Lendor is giving me a trial to
+become a toolsmith. Let's check out the
+toolsmithing equipment and actually try tool
+smithing.</t>
   </si>
   <si>
     <t xml:space="preserve">氷の領界のイーサの村にいる　リルチェラから
@@ -176,6 +337,14 @@
 恵みの木の裏側を　調べてみよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Lilcherat, who is in the Ether Village of the
+Ice Realm, has a problem and would like you
+to consult with him! A mysterious voice came
+out of nowhere and told me to check the back
+side of Grace Tree, so please follow me.
+Let's check the backside of Grace Tree.</t>
+  </si>
+  <si>
     <t xml:space="preserve">氷の領界のイーサの村にいる　リルチェラに頼まれ
 恵みの木の裏側を調べると　恵みの木の中にある
 ふしぎな世界　恵みの園で　サジェと再会した。
@@ -184,10 +353,25 @@
 白霜の流氷野の　ダークシルフを倒そう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Lilcherat in the Ether Village of the Ice
+Realm asked me to check the backside of the
+Grace Tree, and I met Sajay again in the
+mysterious world of Gratia inside the Grace
+Tree. I defeated White Imp in the Eternal Ice
+Field and Dark Sylph in the Frosty Ice Field
+to find out the contents of the Sacred Secret
+in the Book of All Things.</t>
+  </si>
+  <si>
     <t xml:space="preserve">港町レンドア南の宿屋にある　鏡の向こうで
 リュナンが　待っている。
 魔法使いになっているなら
 宿屋に泊まって　鏡に話しかけてみよう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunan is waiting for you behind the mirror at
+the inn in South Port Lendor. If you are a
+mage, stay at the inn and talk to the mirror.</t>
   </si>
   <si>
     <t xml:space="preserve">夢幻の森の捨てられた城で　囚われている
@@ -198,6 +382,15 @@
 とどめをさしたときだけ　手に入るらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">Bring me the Safe Pass Stone from Lunan, who
+is being held captive in the Abandoned Castle
+in the Dream Forest, in order to break the
+magic spell! The Safe Pass Stone can only be
+obtained by using Crack to finish off
+Incubus, who appears at night in the Dream
+Forest.</t>
+  </si>
+  <si>
     <t xml:space="preserve">港町レンドア北にある　道具鍛冶ギルドで
 マスター・バレクスから　レベル３１以上の
 道具鍛冶職人になるため　★以上の
@@ -206,33 +399,66 @@
 引き受けてくれ！　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Accept an assignment from Guildmaster Barex
+at the Toolsmith Guild in North Port Lendor
+to create and bring back new Silver Alchemy
+Pot with a ★ or higher to become a level 31+
+toolsmith!</t>
+  </si>
+  <si>
     <t xml:space="preserve">チョッピ荒野の　荒野の休息所で
 ココナという　プクリポの女性が
 美容院で使える　新しい色を作るための
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">A Pukulipo woman named Cocona at the
+Wilderness Retreat in Choppi Wilderness needs
+help creating new colors for use at the
+Salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ブーナー熱帯雨林の　密林の野営地で
 ジェーンという　ウェディの女性が
 美容院で使える　新しい色を作るための
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">At the Jungle Camp in the Booner Rainforest,
+a Weddie woman named Jane needs help creating
+new colors for the Salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">落陽の草原の　ガケっぷち村で
 シズクという　エルフの女性が
 美容院で使える　新しい色を作るための
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">In the Ruined Village of Sunset Meadow, an
+Elf woman named Shizuku is seeking help in
+creating new colors for use in her salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ゴブル砂漠西の　商人たちのテントで
 ドワーフの女の子　ミミルナが
 美容院で使える　新しい色を作るための
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">In the merchants' tents at Goble Desert West,
+Dwarf girl Mimilna needs help creating new
+colors for use at the Salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ギルザッド地方の　入り江の集落で
 バロンという老人が　美容院で使える
 新しい色を作るための　手助けを求めている。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Cove Village, Gilzad Region, an old man
+named Baron needs help creating new colors
+for use in the Salon.</t>
   </si>
   <si>
     <t xml:space="preserve">オルフェア地方東の　ピィピのお宿で
@@ -241,15 +467,30 @@
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">At Pipi's Inn in Orphea Region East, a
+Pukulipo woman named Mamapona is seeking help
+in creating new colors for use at the Salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">アズラン地方の　木かげの集落で
 ヤツハという　エルフの女性が
 美容院で使える　新しい色を作るための
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">In Treeshade Village, Azlan Region, an Elf
+woman named Yatsuha is seeking help in
+creating new colors for her salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">獅子門の集落で　ガモという　オーガの女性が
 美容院で使える　新しい色を作るための
 手助けを求めている。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At Lion Gate Village, an Ogre woman named
+Gamo needs help creating new colors for the
+Salon.</t>
   </si>
   <si>
     <t xml:space="preserve">モガリム街道の　モガレキャンプで
@@ -258,9 +499,19 @@
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">At Mogare Camp on Mogarim Highway, a Dwarf
+woman named Lorod is asking for help in
+creating new colors for use at the Salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">風の町アズランの　アズラン温泉にいる
 エルフの女性　マンジュが
 レベル２２以上の旅人を　探しているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manju, an Elf woman at the Azlan warm
+fountain in Wind Town Azlan, is looking for
+travelers of level 22 and above.</t>
   </si>
   <si>
     <t xml:space="preserve">港町レンドア北にある　教会で
@@ -270,14 +521,31 @@
 彼の気持ちに　応えられるかもしれない。</t>
   </si>
   <si>
+    <t xml:space="preserve">Rigado, who trains adventurers at the Church
+in North Port Lendor, is looking for the
+right person. Adventurers with a prestige
+level of 25 or above may be able to
+accommodate him.</t>
+  </si>
+  <si>
     <t xml:space="preserve">イナミノ街道の　山間の関所の　片隅で
 ヒガンという　元美容師の　エルフの女性が
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">In a corner of Mountain Pass on the Inamino
+Highway, an Elf woman named Higan, a former
+hairdresser, is asking for help.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ゲルト海峡の　宿屋の前で
 バラバという　美容師見習いの　オーガの女性が
 手助けを求めている。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An Ogre woman named Baraba, an apprentice
+hairdresser, asks for help in front of an inn
+on Gert Strait.</t>
   </si>
   <si>
     <t xml:space="preserve">キラキラ大風車塔の　カフェテラスで
@@ -286,9 +554,19 @@
 手助けを求めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">Pukulipo man Puchino, manager of Salon Fe
+Lycia, needs help at Cafe Terrace in Glitter
+Windmill Tower.</t>
+  </si>
+  <si>
     <t xml:space="preserve">グランゼドーラ王国　美容院にいる
 美容師の女性　ヴィタルが
 手助けを求めているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems that Vitar, a female hairdresser at
+the Gran Zedora Kingdom Salon, needs some
+help.</t>
   </si>
   <si>
     <t xml:space="preserve">聖都エジャルナにいる　竜族の男性
@@ -297,20 +575,40 @@
 興味を持っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Ignorant Guru Izola, a dragon man in Holy
+City Ejarna, is interested in anyone above
+level 90 who wants to become more powerful.</t>
+  </si>
+  <si>
     <t xml:space="preserve">メギストリスの都の　噴水公園下にいる
 プクリポの男性　プッツンが
 カモを探しているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Pukulipo man Puttsun at the below fountain in
+City of Megistris is looking for ducks.</t>
+  </si>
+  <si>
     <t xml:space="preserve">偽りのグランゼドーラ王国にいる
 派手な服装で　特徴的なヒゲの　男性が
 話を聞いてくれる冒険者を　探しているらしい。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A man in the false Gran Zedora Kingdom,
+dressed in fancy clothes and with a
+distinctive beard, is apparently looking for
+an adventurer who will listen to him.</t>
   </si>
   <si>
     <t xml:space="preserve">ガートラント城１階　炎の間にいる
 オーガの男性　ジウバが
 レベル５０以上の冒険者に
 何か　頼みごとがあるようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jiuba, an Ogre man at The Flame on the first
+floor of Gartlant Castle, has a request for
+adventurers above level 50.</t>
   </si>
   <si>
     <t xml:space="preserve">＼＼★無料キャンペーンのご案内★／／
@@ -321,6 +619,15 @@
 グランゼドーラ王国宿屋　担当者リンクス</t>
   </si>
   <si>
+    <t xml:space="preserve">Free Kyan Pennies★/ / / The first one to get
+in early wins!　Limited number of
+people!　First come, first served! We are now
+offering a completely free Kyan Pane to make
+Mega Zoomstone even more convenient! ↓Contact
+us for more information ↓ Gran Zedora Kingdom
+Innkeeper Contact Person Lynx</t>
+  </si>
+  <si>
     <t xml:space="preserve">ジュレットの町にいる
 ウェディの男性　レテリオが
 レベル１０以上の旅人に
@@ -329,8 +636,18 @@
 求めている……らしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">It appears that Reterio, a Weddie male in
+Julet Town, is asking for help from level 10+
+travelers. Apparently a hungry wolf is asking
+for a battle dress set .......</t>
+  </si>
+  <si>
     <t xml:space="preserve">ドルワーム王国の民家にいる　ヘチャブが
 何か　困っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hechab in the Dolworm Kingdom house seems to
+be in some kind of trouble.</t>
   </si>
   <si>
     <t xml:space="preserve">港町レンドア駅の　売店の前にいる
@@ -338,9 +655,19 @@
 手助けを求めているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Shirotsume, the Elf woman in front of the
+Port Town Lendor Stop shop, seems to be
+asking for help.</t>
+  </si>
+  <si>
     <t xml:space="preserve">娯楽島ラッカランの宿屋にいる　老人の２人組
 モバーと　イールが　お客様の訪れを
 待っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems that Moe and Byle, a couple of old
+men at an inn on Luckland Island, are waiting
+for their guests to visit.</t>
   </si>
   <si>
     <t xml:space="preserve">素材屋に　上がりにくかった部位の　使い込み度が 
@@ -350,11 +677,24 @@
 １０回　勝利してきてください！　と言われた。</t>
   </si>
   <si>
+    <t xml:space="preserve">For a convenient way to increase the
+usability of a hard-to-get-up item in the
+Material Shop, equip yourself with the
+Material Shop Red Cap and win 10 battles
+against the demons in Moncello Spring Gorge!</t>
+  </si>
+  <si>
     <t xml:space="preserve">ガートラント城にいる　ジウバに
 バグレア教会跡地で　神父の幽霊が
 嘆き悲しんでいる夢を　よく見るので
 様子を見てきてほしい！　と頼まれた。
 グレン領西にある　バグレア教会跡地に向かおう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jiuba at Gartlant Castle often dreams of the
+ghost of a priest mourning at Bagulea Church
+Vestige, so please go check on him! Let's
+head to Bagulea Church Vestige in Glen West.</t>
   </si>
   <si>
     <t xml:space="preserve">嵐の領界のムストの町で　魔法生物ニコちゃんに
@@ -365,6 +705,14 @@
 連れていこう！</t>
   </si>
   <si>
+    <t xml:space="preserve">Do me a favor and grant the magical creature
+Smyles a wish in the Town of Must in the
+Storm Realm! Take Smyles to the place where
+the Flame Tree grows to see if the rumors of
+plants in the other realms are true, as told
+to me by the Knights of the Gale!</t>
+  </si>
+  <si>
     <t xml:space="preserve">ガートラント城にいる　ジウバに頼まれて
 バグレア教会跡地の　神父の幽霊を訪ねてみた。
 神父が探している子供の幽霊　ブリックを
@@ -373,6 +721,15 @@
 直し方は　ガミルゴが　知っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Jiuba in Gartlant Castle asked me to visit
+the ghost of the priest of Bagulea Church
+Vestige. When I found Brick, the ghost of the
+child the priest was looking for, Brick told
+me that he had broken an idol in the church
+and wanted me to fix it. Gamilgo seems to
+know how to fix it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">バグレア教会跡地にいる幽霊　オッド神父が
 探していた　子供の幽霊　ブリックは
 教会にあった　神像を　壊してしまったので
@@ -381,6 +738,15 @@
 バグレア教会跡地に行き　オッド神父に渡そう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Father Od, a ghost in Bagulea Church Vestige,
+is looking for Brick, a ghost of a child, who
+has broken an idol in the church and wants it
+fixed. Since Gamilgo fixed the idol in the
+past world, let's go to Bagulea Church
+Vestige in Glen West and give it to Father
+Od.</t>
+  </si>
+  <si>
     <t xml:space="preserve">子供の幽霊　ブリックが　壊してしまった
 神像を　ガミルゴに　直してもらい
 オッド神父に渡すと　ブリックは　天へ
@@ -389,6 +755,12 @@
 ガートラント城の　ジウバに　報告しにいこう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Brick's idol was broken by a child ghost,
+Brick, and when Gamilgo fixed it and gave it
+to Father Od, Brick was led up to heaven.
+Let's report to Jiuba at Gartlant Castle.</t>
+  </si>
+  <si>
     <t xml:space="preserve">氷の領界のイーサの村にいる　ヒヤーネに頼まれ
 リルチェラに贈るふとん作りを　手伝うことに。
 そのため　白霜の流氷野の　大魔獣イーギュアを
@@ -397,6 +769,15 @@
 現在　ホンワカ羽毛を　０個　集めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">Hyane in Ether Village in the Ice Realm asked
+me to help him make a futon for Lilcherat. To
+do so, he asked me to help him defeat the
+Giga Rapscallion in the Frosty Ice Field or
+collect 200 feathers dropped by the Polar
+Polly. Currently, he has collected 0 Honwaka
+Feathers.</t>
+  </si>
+  <si>
     <t xml:space="preserve">落陽の草原の　ガケっぷち村で　シズクから
 美容院で使える新しい色を作るために
 呪われた大地の　ウドラーが落とす
@@ -404,6 +785,12 @@
 と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Shizuku at Ruined Village in Sunset Meadow
+would like to get some Enchanted Grapes from
+Treevil in Cursed Land to make new colors for
+the salon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ゴブル砂漠西の　商人たちのテントで　ミミルナに
 美容院で使える　新しい色を作るため
 ボロヌス溶岩流の　ベホマスライムが
@@ -411,6 +798,13 @@
 手に入れてほしいんですの！　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">I need Mimilna at the merchants' tents in
+Goble Desert West to get some Lava Berries
+that Cureslime from Boronus Lava Flow
+sometimes drops to make new colors for the
+salon!</t>
+  </si>
+  <si>
     <t xml:space="preserve">ギルザッド地方の　入り江の集落で　バロンから
 美容院で使える新しい色を作るために
 トガス岩道で　ヘルコンダクターと手合わせし
@@ -418,11 +812,24 @@
 手に入れてきていただけますかな？　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Would you be willing to meet with Hell
+Conductor on Togas Rock Road at Cove Village
+in the Gilzad Region to create a new color
+for the salon from Baron and get us what we
+would call a Gentleman's Taste?</t>
+  </si>
+  <si>
     <t xml:space="preserve">グレン城の１階にある　訓練場で
 オーガの男性　教官ランババが
 鍛える相手を探しているようだ。
 レベル５０以上の　冒険者ならば
 彼の特訓を　受けられるだろう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ogre male instructor Ranbaba is looking for
+someone to train at the training grounds on
+the first floor of Glen Castle. Adventurers
+of level 50 or above can take his training.</t>
   </si>
   <si>
     <t xml:space="preserve">オルフェア地方東の　ピィピのお宿で
@@ -433,6 +840,13 @@
 手に入れてきて～ん！　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">I need to get the Night Whisper that is
+sometimes dropped by the Invisible Swordsman
+of Sage's Lair in Popola Region to make a new
+color for the Salon from Mamapona at Pipi's
+Inn in Orphea Region East!</t>
+  </si>
+  <si>
     <t xml:space="preserve">アズラン地方の　木かげの集落で　ヤツハから
 美容院で使える新しい色を作るために
 アズラン地方の　南東の川沿いにいる
@@ -440,6 +854,13 @@
 取り返してきてもらえまへん？　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Can you please go to Treeshade Village in
+Azlan Region and get back the Tea Plant
+Leaves from the Tranquilander along the
+southeast river in Azlan Region so that
+Yatsuha can create new colors for the Salon?</t>
+  </si>
+  <si>
     <t xml:space="preserve">獅子門の集落にいる　ガモから
 美容院で使える　新しい色を作るために
 ランガーオ山地の　南部や　東部にいる
@@ -447,13 +868,28 @@
 お願いできないかい？　と頼まれた。</t>
   </si>
   <si>
+    <t xml:space="preserve">Can you get Pure White Snow from Frostburn in
+the southern and eastern Langao Mountains
+from Gamo in Lion Gate Village to make a new
+color for Salon?</t>
+  </si>
+  <si>
     <t xml:space="preserve">エテーネの村にいる　シンイが
 セラニーを　待っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems that Shini in Ethene Village is
+waiting for Serany.</t>
   </si>
   <si>
     <t xml:space="preserve">オルフェアの町にいる　プクリポの女性
 プールプが　レベル１０以上の旅人に
 何か頼みたいことが　あるようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulup, a Pukulipo woman in the Town of
+Orphea, has a request for travelers of level
+10 and above.</t>
   </si>
   <si>
     <t xml:space="preserve">岳都ガタラの中央広場で
@@ -462,10 +898,21 @@
 手助けを求めているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">At the Center Plaza in Mount Gatara, Lerena,
+a Dwarf woman, appears to be asking for help
+from travelers level 10 and above.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ゲルト海峡の　宿屋前で　バラバに
 ゲルト海峡にいる　たてまじんから
 死んだダチの形見の
 落日のフラッグを取り戻してくれ！　と頼まれた。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In front of the inn in Gert Strait, ask
+Baraba to retrieve the Sunset Flag, a memento
+of my dead friend, from Peekabogre in Gert
+Strait!</t>
   </si>
   <si>
     <t xml:space="preserve">キラキラ大風車塔で　プチーノから
@@ -475,6 +922,12 @@
 ０個　集めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">I got 10 3-Star Blend Beans back from Puchino
+in Glitter Windmill Tower, which were stolen
+by the monsters on Windmill Way! I currently
+have 0 3-Star Blend Beans.</t>
+  </si>
+  <si>
     <t xml:space="preserve">キラキラ大風車塔で　プチーノから
 風車の丘の　モンスターたちに奪われた
 三つ星ブレンド豆を　１０個　取り返して！
@@ -482,6 +935,12 @@
 ３個　集めている。</t>
   </si>
   <si>
+    <t xml:space="preserve">I got 10 3-Star Blend Beans back from Puchino
+in Glitter Windmill Tower, which were stolen
+by the monsters on Windmill Way! I have 3
+3-Star Blend Beans now.</t>
+  </si>
+  <si>
     <t xml:space="preserve">グランゼドーラ王国の　美容院にいる
 ヴィタルに　新色ヘアカラー追加のために
 サラツヤオイルを手に入れて！　と頼まれた。
@@ -489,8 +948,18 @@
 プークプックが　落とすらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">Get Glossy Oil from Vitar at the Salon in
+Gran Zedora Kingdom to add a new hair color!
+Glossy Oil is said to be dropped by Satyr in
+Gran Zedora Territory.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ツスクルの村にいる　エルフの女性
 テマリが　何か　困っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temari, an Elf woman in Tsusukul Village,
+seems to be in some kind of trouble.</t>
   </si>
   <si>
     <t xml:space="preserve">炎の領界　聖都エジャルナの大神殿の２階
@@ -498,13 +967,28 @@
 セラニーの訪れを　待っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">The priest Besawaki in front of Estella's
+Room on the second floor of the Great Temple
+in Fire Realm Holy City Ejarna seems to be
+waiting for Serany's visit.</t>
+  </si>
+  <si>
     <t xml:space="preserve">グレン城下町駅にいる　オーガの男性
 マイラーの　ギオーダが
 何か　頼みごとがあるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Gioda, the Ogre male miler at the Glen Castle
+Town Stop, seems to have a favor to ask.</t>
+  </si>
+  <si>
     <t xml:space="preserve">嵐の領界のムストの町の地下　下層にいる
 イルギ町長が　何か　困っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayor Irugi in the lower level of the Town of
+Must in the Storm Realm seems to be in some
+kind of trouble.</t>
   </si>
   <si>
     <t xml:space="preserve">水の領界の　海底都市ルシュカにいる
@@ -512,12 +996,26 @@
 何か　頼みごとがあるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Burg, a dragon man in the City of Ruska in
+the Water Realm, seems to have a favor to
+ask.</t>
+  </si>
+  <si>
     <t xml:space="preserve">水の領界のカシャル海底神殿にいる
 青の騎士団員のテトが　何か　困っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Tet, a member of the Blue Knights at the
+Kashal Submarine Temple in Water Realm, seems
+to be in some kind of trouble.</t>
+  </si>
+  <si>
     <t xml:space="preserve">闇の領界の　カーラモーラ村で
 カイラム村長が　何か困っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chief Kairam is in trouble at Carlamora
+Village in the Dark Realm.</t>
   </si>
   <si>
     <t xml:space="preserve">炎の領界の　聖都エジャルナにいる
@@ -525,31 +1023,63 @@
 何か　困っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Ioma, a dragoness in Holy City Ejarna in the
+Fire Realm, seems to be in some kind of
+trouble.</t>
+  </si>
+  <si>
     <t xml:space="preserve">闇の領界の　カーラモーラ村にいる
 バジューの妹　ミルテが
 頼みごとがあるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Baju's sister Mirta in Carlamora Village in
+the Dark Realm has a favor to ask.</t>
+  </si>
+  <si>
     <t xml:space="preserve">氷の領界のイーサの村にいる
 竜族のおばあさん　ヘモニグが
 何か　頼みごとがあるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Hemonig, a dragon grandmother in the Ice
+Realm's Ether Village, seems to have a favor
+to ask.</t>
+  </si>
+  <si>
     <t xml:space="preserve">炎の領界の　アペカの村にいる
 竜族のおじいさん　エーゴンが
 何か　困っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Agon, the old man of the dragon tribe in
+Apeka Village in the Fire Realm, seems to be
+in some kind of trouble.</t>
+  </si>
+  <si>
     <t xml:space="preserve">竜族の隠れ里にいる老人　ゴハから
 何か　頼みごとがあるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">It seems that Goha, an old man at Nadravian's
+Rest, has a favor to ask.</t>
+  </si>
+  <si>
     <t xml:space="preserve">炎の領界のアぺカの村にいる　ネオル村長が
 何か　困っているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Chief Neoru in the village of Apeca in the
+Fire Realm seems to be in some kind of
+trouble.</t>
+  </si>
+  <si>
     <t xml:space="preserve">聖都エジャルナの郵便局で
 便せん屋ミカゲが　手助けを求めている。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper Shop Mikage needs help at the Post
+Office in Holy City Ejarna.</t>
   </si>
   <si>
     <t xml:space="preserve">グランゼドーラ王国にいる　リンクスから
@@ -560,6 +1090,12 @@
 資料室に　置いてあるらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">I need to get Holy Powder from Lynx in Gran
+Zedora Kingdom to upgrade Mega Zoomstone!
+Holy Powder is said to be in locked Archives
+in the southeast of Celedot Mountain Pass.</t>
+  </si>
+  <si>
     <t xml:space="preserve">グランゼドーラ王国にいる　リンクスから
 メガルーラストーンをグレードアップするため
 ホーリーパウダーを　取ってきてほしい！
@@ -568,6 +1104,12 @@
 ヘルビーストが　落とすらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">I need to get Holy Powder from Lynx in Gran
+Zedora Kingdom to upgrade Mega Zoomstone! I
+found out from Archives that Holy Powder is
+dropped by Sculptrice in Solaria Canyon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">グランゼドーラ王国にいる　リンクスから
 メガルーラストーンを　グレードアップするため
 ホーリーパウダーを　取ってきてほしい！
@@ -576,9 +1118,21 @@
 リンクスの所へ持っていこう。</t>
   </si>
   <si>
+    <t xml:space="preserve">I need you to get Holy Powder from Lynx in
+Gran Zedora Kingdom to upgrade Mega
+Zoomstone! I received Holy Powder at the
+false Solaria Canyon, so let's take it to
+Lynx.</t>
+  </si>
+  <si>
     <t xml:space="preserve">グランゼドーラ王国　美容院にいる
 美容師の女性　ヴィタルが
 また　手助けを求めているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems that Vitar, the hairdresser lady at
+the Gran Zedora Kingdom Salon, needs another
+helping hand.</t>
   </si>
   <si>
     <t xml:space="preserve">預かり所の従業員に　入会の手続きのため
@@ -589,6 +1143,14 @@
 預かり所が　使えるようになった！</t>
   </si>
   <si>
+    <t xml:space="preserve">I want an employee of the Depository to bring
+me the Glittering Ink that Bubble Slime drops
+to complete the enrollment process! I signed
+the application form with the received
+Glittering Ink, and the Depository is now
+ready to use it!</t>
+  </si>
+  <si>
     <t xml:space="preserve">預かり所の従業員に　新しい倉庫の
 性能テストのため　つけもの石
 上やくそう　まほうの小ビンを
@@ -597,14 +1159,33 @@
 お礼として　新しい倉庫が使えるようになった。</t>
   </si>
   <si>
+    <t xml:space="preserve">An employee of the depository asked me to
+bring a specified number of Flintstone Strong
+Medicine Single Phials to test the
+performance of the new storage!　I
+accomplished this. In return, the new storage
+became available.</t>
+  </si>
+  <si>
     <t xml:space="preserve">真のセレドット山道の資料室にいる
 ナゾの人物が　旅人の訪れを
 待っているらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">A mysterious figure in the Archives of true
+Celedot Mountain Pass is apparently waiting
+for travelers to visit.</t>
+  </si>
+  <si>
     <t xml:space="preserve">辺境警備隊詰所にいる兵士　ヘキートに
 詰所の近くに出る魔物に盗まれた　大事なモンを
 取り返してくれねえか？　と頼まれた。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I asked Hequito, a soldier at the Frontier
+Guard Post, if he could return a valuable
+item that was stolen by a monster that
+appears near the guard post.</t>
   </si>
   <si>
     <t xml:space="preserve">港町レンドア南で　詩人ナスガルドから
@@ -614,15 +1195,33 @@
 勝利を誓うように　言われた。</t>
   </si>
   <si>
+    <t xml:space="preserve">In South Port Lendor, Poet Woebergard
+explained the rules of warfare necessary to
+set the stage for the War Poem of
+Cucumberserk. You were then told to use the
+emote "Guts Pose" and pledge victory.</t>
+  </si>
+  <si>
     <t xml:space="preserve">真のグランゼドーラ王国にいる　人間の男性
 シルベッスが　いずれかの職業のレベルが
 １２８に到達した冒険者を　待っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A man named Silbess is waiting for
+adventurers of at least level 128 in
+the true Gran Zedora Kingdom.</t>
   </si>
   <si>
     <t xml:space="preserve">オーグリード大陸　ラギ雪原の西にある
 竜術士の家に住んでいる　ランジェが
 待っているようだ。
 竜術士に転職して　行ってみよう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranje, who resides in the Dragomancer's
+House in the Ragi Snowfield in Ogreed,
+is waiting for you. Go here to learn how
+to become a Dragomancer.</t>
   </si>
   <si>
     <t xml:space="preserve">メネト村にいる　ミミッタから頼まれ　ティセを
@@ -633,6 +1232,14 @@
 天使のチカラを宿す液体を入手し　花にかけよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">At the request of Mimitta in Menet Village, she
+wants cheer up Tise by making a flower crown. You
+ask Pepinora for the location of Tohpes' flowers
+and go outside town, but the flowers had withered.
+A mysterious voice said they would bloom again
+with liquid imbued with angelic power.</t>
+  </si>
+  <si>
     <t xml:space="preserve">王都カミハルムイのレンジャー協会本部から
 モリナラ支部に　派遣された。
 支部長ポランパンから　先輩のユウギリと共に
@@ -641,6 +1248,14 @@
 先に森の奥へ行った　ユウギリに追いつこう。</t>
   </si>
   <si>
+    <t xml:space="preserve">I was sent to Molinara branch from Ranger
+Association HQ in Kamiharmui City. Poranpan, the
+branch manager, asked me to work with Yugiri, his
+senior, to deal with the Guaardvark that was
+destroying the forest! to do something about the
+Guaardvark that is ravaging the forest. [...]</t>
+  </si>
+  <si>
     <t xml:space="preserve">レンジャー協会モリナラ支部での　初仕事。
 先輩のユウギリから　森を荒らしている
 スカルガルーを　５匹
@@ -649,6 +1264,14 @@
 無効らしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">My first job in the Molinara branch of the Ranger
+Association. Yugiri, my senior, asked me to
+release five Guaardvarks that were tearing up the
+forest using Mercy! I was asked to use Mercy to
+release five Guaardvarks that were ravaging the
+forest. I was told that any misses are not [...]</t>
+  </si>
+  <si>
     <t xml:space="preserve">エルトナ・レンジャー協会　モリナラ支部で
 ポランパン支部長から　レーノスと共に
 モリナラ大森林の木を　勝手に切り倒している
@@ -657,6 +1280,14 @@
 モリナラ大森林の奥を　徹底的に調査しよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Poranpan, the president of the Eltona Ranger
+Association Molinara Chapter, asked me to work
+with Renosu to find the illegal loggers who are
+cutting down trees in the Molinara Forest without
+permission! Renosu challenged me to find the
+culprits by myself.</t>
+  </si>
+  <si>
     <t xml:space="preserve">エルトナ・レンジャー協会　モリナラ支部で
 ポランパン支部長から　伐採同盟に囚われた
 ユウギリを　助けだしてほしい！　と頼まれた。
@@ -664,6 +1295,14 @@
 レーノスと共に　向かおう。</t>
   </si>
   <si>
+    <t xml:space="preserve">I was asked by Poranpan, head of the Eltona
+Ranger Association's Molinarra branch, to help
+rescue Yugiri, who was being held captive by a
+logging alliance! Yugiri is trapped by the
+logging alliance. Let's go with Renosu to the
+Outer Forest Cave where the alliance [...]</t>
+  </si>
+  <si>
     <t xml:space="preserve">森の怒りを鎮めるには　レンジャーの必殺技を
 習得しなければ　ならないらしい。
 そのための試練として　落陽の草原などで
@@ -671,11 +1310,24 @@
 と言われた。</t>
   </si>
   <si>
+    <t xml:space="preserve">To appease the wrath of the forest, it seems that
+you must master the ranger's special move. To do
+so, I was told to go to Sunset Meadow and kill
+five Bud Brothers as a trial! I was told.</t>
+  </si>
+  <si>
     <t xml:space="preserve">レンジャーの必殺技　妖精たちのポルカを
 身につけるために　まだらイチョウを
 ５匹　倒してこい！　と言われた。
 すでに　５匹倒し　試練を達成した。
 レンジャー協会本部に　戻ろう。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was told to kill 5 Bud Brother in order to
+learn the ranger's special move Brownie Boost!
+I've already killed 5 of them and completed the
+trial. I've already killed 5 and completed the
+trial.</t>
   </si>
   <si>
     <t xml:space="preserve">モリナラ支部のポランパン支部長から
@@ -686,11 +1338,27 @@
 勝たなくてはならないらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">Poranpan, the head of the Molinara branch, asked
+me to kill the Tree of Hatred in the Green
+Sanctuary deep in the Molinara Forest to appease
+the forest's anger and save the people who have
+been turned into monsters! to save the people who
+have been turned into monsters. In this [...]</t>
+  </si>
+  <si>
     <t xml:space="preserve">娯楽島ラッカランのササラナに　整理術のために
 本の下巻を探してほしい！　と頼まれた。
 ササラナに　本が見つからなかったことを伝えると
 整理術の開発は　手元の上巻でなんとかするから
 タバネのチカラになって！　と言われた。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sasalana from Luckland Island asked me to find
+the bottom volume of the book for her
+organizational skills! When I told Sasalana that
+I couldn't find the book, she told me that she
+would help Tabane in the development of the
+organizing system, since she had the upper [...]</t>
   </si>
   <si>
     <t xml:space="preserve">娯楽島ラッカランのササラナに　タバネのチカラに
@@ -701,11 +1369,25 @@
 行くには　ハシバミと話せば　いいようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Sasalana in Luckland Island asked me to help
+Tabane! I talked to Hashibami, Tabane's father,
+who is in the inn in Wind Town Azlan, and he was
+worried that her sister Chihiro had not come back
+home, so we decided to look for clues.</t>
+  </si>
+  <si>
     <t xml:space="preserve">謎の異空間にいる　世告げの姫ロディアから
 帝王の玉座に掛かっている幻術を解く時が
 来たので　闇の溢る世界に向かうよう
 言われた。帝王の玉座にいる　災厄の王は
 幻影であり　もう一度　戦うことになるらしい。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Princess of ProphecyRhodia, who is in a
+mysterious foreign space, told me to go to the
+World of Darkness because it was time to break
+the spell on the Imperial Throne. I will have to
+fight him again.</t>
   </si>
   <si>
     <t xml:space="preserve">娯楽島ラッカランのササラナに　タバネのチカラに
@@ -716,28 +1398,62 @@
 提案した。ササラナのところへ　行こう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Sasalana from Luckland Island asked me to help
+Tabane! When Chihiro told him what had happened,
+Tabane suggested that he should talk to Sasalana
+about his sister's room.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 {color=yellow}強戦士の聖域・闘場{reset}にいる
 {color=yellow}魔軍師イッド強{reset}を　１匹　討伐してほしい！
 現在　０匹　倒している。</t>
   </si>
   <si>
+    <t xml:space="preserve">Request from Monster Strike Force member
+{color=yellow}I want you to take out one
+{color=yellow}Apex Tactician Idd{reset} in
+Warrior's Sanctuary - Arena{reset}! Currently, 0
+of them have been killed.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 {color=yellow}強戦士の聖域・闘場{reset}にいる
 {color=yellow}呪術師マリーン強{reset}を　１匹　討伐してほしい！
 現在　０匹　倒している。</t>
   </si>
   <si>
+    <t xml:space="preserve">Request from Monster Strike Force member
+{color=yellow}I need you to kill 1
+{color=yellow}Apex Monstrous Malynn in Warrior's
+Sanctuary - Arena {reset}! He has killed 0 so
+far.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 {color=yellow}強戦士の聖域・闘場{reset}にいる
 {color=yellow}暴君バサグランデ強{reset}を　１匹　討伐してほしい！
 現在　０匹　倒している。</t>
   </si>
   <si>
+    <t xml:space="preserve">Request from Monster Strike Force member
+{color=yellow}I want you to take out one
+{color=yellow}Apex Tyrant Bogan{reset} in
+Warrior's Sanctuary - Arena{reset}! Currently, 0
+of them have been killed.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 {color=yellow}強戦士の聖域・闘場{reset}にいる
 {color=yellow}魔人エンラージャ強{reset}を　１匹　討伐してほしい！
 現在　０匹　倒している。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request from Monster Strike Force member
+{color=yellow}I want you to kill one
+{color=yellow}Apex Enraja{reset} in Warrior's
+Sanctuary - Arena{reset}! Currently, 0 have been
+killed.</t>
   </si>
   <si>
     <t xml:space="preserve">ジュレットの町にある　さいほうギルドで
@@ -747,16 +1463,37 @@
 持ってきてほしい！　と言われた。</t>
   </si>
   <si>
+    <t xml:space="preserve">At the Sewing Guild in Julet, Guildmaster Yubia
+asked me to make  or higher Holy Boots and bring
+them to him as new boots in order to become a
+Level 46+ Sewer! He asked me to bring him a new
+pair of boots.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 {color=yellow}強戦士の聖域・闘場{reset}にいる
 {color=yellow}天魔クァバルナ強{reset}を　１匹　討伐してほしい！
 現在　０匹　倒している。</t>
   </si>
   <si>
+    <t xml:space="preserve">Request from Monster Strike Force member
+{color=yellow}To kill 1 {color=yellow}Apex
+Kukulkannibal{reset} in {color=yellow}Book of
+Bosses - Arena{reset}! Currently, 0
+Kukulkannibals have been defeated.</t>
+  </si>
+  <si>
     <t xml:space="preserve">～モンスター討伐隊隊員からの依頼～
 {color=yellow}強戦士の聖域・闘場{reset}にいる
 {color=yellow}悪魔長ジウギス{reset}を　１匹　討伐してほしい！
 現在　０匹　倒している。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request from Monster Strike Force member
+{color=yellow}To defeat one {color=yellow}Devil
+Chief Jiggis{reset} in the Book of Bosses -
+Arena{reset}! Currently, 0 of them have been
+defeated.</t>
   </si>
   <si>
     <t xml:space="preserve">グランゼドーラ城にいる　賢者ルシェンダから
@@ -767,6 +1504,13 @@
 古き神の遺跡に　向かったらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">Sage Lushenda at Gran Zedora Castle asked me to
+protect Anlucia, who was on her way to defeat the
+demons alone! Anlucia heard that Marshal Zeldrad
+had appeared and headed for the Historic Ruins in
+the depths of Solaria Canyon.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ダーマ神殿にいる　ディエゴから
 スキルポイントの割り振り上限を
 ２００まで　解放するための試練を
@@ -775,6 +1519,14 @@
 加護を受け　試練の舞台へ　飛ばしてもらおう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Diego at Alltrades Abbey asked me if I would take
+a trial to open up my skill point allotment to
+200. He asked me if I was ready to fight. When
+you are ready to fight, ring the bell of
+destruction outside the temple, in front of the
+entrance, to receive blessings and be [...]</t>
+  </si>
+  <si>
     <t xml:space="preserve">謎の異空間にいる　世告げの姫サテラから
 災厄の王の幻術を打ち破るために
 自分の封じられた記憶を　取り戻してほしい！
@@ -783,6 +1535,14 @@
 覚えているらしい。その子を探して話を聞こう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Princess of ProphecySatella, who lives in a
+mysterious alien space, asks you to retrieve her
+sealed memories in order to defeat the King of
+Calamity's illusions! Satella seems to remember a
+girl in a big church in a port town somewhere in
+her dim memory. Let's find her and talk to her.</t>
+  </si>
+  <si>
     <t xml:space="preserve">港町レンドア南で　詩人ナスガルドから
 ベジセルクの戦詩を紡ぐ　舞台作りに必要な
 もうひとつのピースである　黄昏の詩人の楽譜を
@@ -791,8 +1551,20 @@
 アモデウスを倒すと　手に入るらしい。</t>
   </si>
   <si>
+    <t xml:space="preserve">I was asked by Poet Woebergard in South Port
+Lendor to get Twilight Poet's Score, which is
+another Peace needed to set the stage for
+Cucumberserk's war poetry! I heard that you can
+get it by defeating Amodeus at Popolia Mushroom
+Mountain and other places in Pukuland.</t>
+  </si>
+  <si>
     <t xml:space="preserve">偽りのメルサンディ村で
 吟遊詩人パニーノが　困っているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F. In Melsandy Village, the bard Panino seems to
+be in trouble.</t>
   </si>
   <si>
     <t xml:space="preserve">オルフェア地方東の　ピィピのお宿にいる
@@ -800,18 +1572,37 @@
 到達した旅人を　探しているようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Elf F sex Light Guide Nazuna at Pippi's Inn in
+Orphea Region East is looking for travelers who
+have reached level 81.</t>
+  </si>
+  <si>
     <t xml:space="preserve">娯楽島ラッカランの　オーナーの館にいる
 ササラナが　レベル７８以上の　冒険者に
 相談したいことが　あるようだ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Sasalana at the Owner's Mansion on Luckland
+Island has some advice for adventurers level 78
+and above.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ガートラント城下町の　井戸の底にいる
 かばん職人パックが　何か困っているようだ。
 職業レベルが８０以上なら　話を聞いてあげよう。</t>
   </si>
   <si>
+    <t xml:space="preserve">If your location level is 80 or higher, we will
+listen to you.</t>
+  </si>
+  <si>
     <t xml:space="preserve">港町レンドア駅の３階にいる　人間の男性
 ペリッツが　冒険者を　探しているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The human man Peritz on the third floor of Port
+Lendor Station seems to be looking for
+adventurers.</t>
   </si>
   <si>
     <t xml:space="preserve">オルフェア地方東　ピィピのお宿にいる
@@ -822,12 +1613,28 @@
 と頼まれた。ナズナに　慈愛を示そう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Light Guide Nazuna at Orphea Region East Pippi's
+Inn will give you the Crest of Kindness, which
+you can get by defeating King Cureslime at
+Popolia Mushroom Mountain and other locations to
+release the level 85 limit. Nazuna asked me to
+take back the Crest of Kindness! Let's show [...]</t>
+  </si>
+  <si>
     <t xml:space="preserve">グランゼドーラ城の　秘密会議室の装置を
 修理できる技師　バジェオと再会した。
 バジェオから　修理に必要な　魔光レンズを
 ラギ雪原の北西などにいる
 キラーマシンから　手に入れ
 直接　秘密会議室に届けてくれ！　と頼まれた。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I met Bajeo again, the technician who can repair
+the equipment in the Secret Meeting Room of Gran
+Zedora Castle. Bajeo asked me to get the Magic
+Lens needed for the repair from the Killing
+Machine northwest of Ragi Snowfield! He asked me
+to deliver it directly to the Secret [...]</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +2047,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:C127"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="80.7109375" customWidth="1"/>
@@ -1254,1012 +2061,1390 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="C66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="C68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="C69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="C70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="C71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="C72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="C73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="C74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="C75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="C76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="C77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="C78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>79</v>
+        <v>156</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="C79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="C80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>81</v>
+        <v>160</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="C81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="C82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="C83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="C84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="C85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="C86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>87</v>
+        <v>172</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="C87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>88</v>
+        <v>174</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="C88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="C89" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="C90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="C91" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="C92" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="C93" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="C94" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="C95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C96" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="C97" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="C98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="C99" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="C100" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="C101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="C102" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>103</v>
+        <v>204</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="C103" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="C104" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="C105" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="C106" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="C107" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>108</v>
+        <v>214</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="C108" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>109</v>
+        <v>216</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="C109" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>110</v>
+        <v>218</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="C110" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>111</v>
+        <v>220</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+      <c r="C111" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="C112" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="C113" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="C114" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="C115" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="C116" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="C117" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>118</v>
+        <v>234</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="C118" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>119</v>
+        <v>236</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="C119" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>120</v>
+        <v>238</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="C120" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>121</v>
+        <v>240</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="C121" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>122</v>
+        <v>242</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="C122" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>123</v>
+        <v>244</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="C123" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>124</v>
+        <v>246</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+      <c r="C124" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>125</v>
+        <v>248</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="C125" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="C126" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>127</v>
+        <v>252</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>127</v>
+        <v>253</v>
+      </c>
+      <c r="C127" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>